<commit_message>
Maps and visualization generated
</commit_message>
<xml_diff>
--- a/Combined.xlsx
+++ b/Combined.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -1333,9 +1333,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>331560</xdr:colOff>
+      <xdr:colOff>331200</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>127440</xdr:rowOff>
+      <xdr:rowOff>127080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1349,7 +1349,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2109600" y="180360"/>
-          <a:ext cx="3782520" cy="3101760"/>
+          <a:ext cx="3782160" cy="3101400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1370,9 +1370,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>425520</xdr:colOff>
+      <xdr:colOff>425160</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1386,7 +1386,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9033120" y="216000"/>
-          <a:ext cx="3782520" cy="3109320"/>
+          <a:ext cx="3782160" cy="3108960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1407,9 +1407,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>399960</xdr:colOff>
+      <xdr:colOff>399600</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>13320</xdr:rowOff>
+      <xdr:rowOff>12960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1423,7 +1423,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2178000" y="3571200"/>
-          <a:ext cx="3782520" cy="3101760"/>
+          <a:ext cx="3782160" cy="3101400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1444,9 +1444,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>298080</xdr:colOff>
+      <xdr:colOff>297720</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>69480</xdr:rowOff>
+      <xdr:rowOff>69120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1460,7 +1460,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8982720" y="3351960"/>
-          <a:ext cx="3705480" cy="3026880"/>
+          <a:ext cx="3705120" cy="3026520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1481,9 +1481,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>414000</xdr:colOff>
+      <xdr:colOff>413640</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:rowOff>73080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1497,7 +1497,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2274480" y="7035840"/>
-          <a:ext cx="3700080" cy="3080520"/>
+          <a:ext cx="3699720" cy="3080160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1518,9 +1518,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>364320</xdr:colOff>
+      <xdr:colOff>363960</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>36360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1534,7 +1534,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9048960" y="7010280"/>
-          <a:ext cx="3705480" cy="3069360"/>
+          <a:ext cx="3705120" cy="3069000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1555,9 +1555,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>425520</xdr:colOff>
+      <xdr:colOff>425160</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:rowOff>163080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1571,7 +1571,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16620840" y="214200"/>
-          <a:ext cx="3782880" cy="3103920"/>
+          <a:ext cx="3782520" cy="3103560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1592,9 +1592,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>298080</xdr:colOff>
+      <xdr:colOff>297720</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>66600</xdr:rowOff>
+      <xdr:rowOff>66240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1608,7 +1608,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16570440" y="3350880"/>
-          <a:ext cx="3705840" cy="3025080"/>
+          <a:ext cx="3705480" cy="3024720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1629,9 +1629,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>364320</xdr:colOff>
+      <xdr:colOff>363960</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>35280</xdr:rowOff>
+      <xdr:rowOff>34920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1645,7 +1645,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16636680" y="7004880"/>
-          <a:ext cx="3705840" cy="3073320"/>
+          <a:ext cx="3705480" cy="3072960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1666,9 +1666,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>426240</xdr:colOff>
+      <xdr:colOff>425880</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>163800</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1682,7 +1682,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="24209640" y="221760"/>
-          <a:ext cx="3782880" cy="3096720"/>
+          <a:ext cx="3782520" cy="3096360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1703,9 +1703,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>298800</xdr:colOff>
+      <xdr:colOff>298440</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1719,7 +1719,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="24159240" y="3351600"/>
-          <a:ext cx="3705840" cy="3018240"/>
+          <a:ext cx="3705480" cy="3017880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1740,9 +1740,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>365040</xdr:colOff>
+      <xdr:colOff>364680</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1756,7 +1756,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="24225480" y="6997320"/>
-          <a:ext cx="3705840" cy="3066840"/>
+          <a:ext cx="3705480" cy="3066480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1777,9 +1777,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>426240</xdr:colOff>
+      <xdr:colOff>425880</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>163800</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1793,7 +1793,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="24209640" y="221760"/>
-          <a:ext cx="3782880" cy="3096720"/>
+          <a:ext cx="3782520" cy="3096360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1814,9 +1814,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>298800</xdr:colOff>
+      <xdr:colOff>298440</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1830,7 +1830,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="24159240" y="3351600"/>
-          <a:ext cx="3705840" cy="3018240"/>
+          <a:ext cx="3705480" cy="3017880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1851,9 +1851,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>365040</xdr:colOff>
+      <xdr:colOff>364680</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1867,7 +1867,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="24225480" y="6997320"/>
-          <a:ext cx="3705840" cy="3066840"/>
+          <a:ext cx="3705480" cy="3066480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1888,9 +1888,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>425520</xdr:colOff>
+      <xdr:colOff>425160</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>163800</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1904,7 +1904,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="31797360" y="221760"/>
-          <a:ext cx="3782880" cy="3096720"/>
+          <a:ext cx="3782520" cy="3096360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1925,9 +1925,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>298080</xdr:colOff>
+      <xdr:colOff>297720</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1941,7 +1941,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="31746960" y="3351600"/>
-          <a:ext cx="3705840" cy="3018240"/>
+          <a:ext cx="3705480" cy="3017880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1962,9 +1962,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>364320</xdr:colOff>
+      <xdr:colOff>363960</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1978,7 +1978,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="31813200" y="6997320"/>
-          <a:ext cx="3705840" cy="3066840"/>
+          <a:ext cx="3705480" cy="3066480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1999,9 +1999,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>425520</xdr:colOff>
+      <xdr:colOff>425160</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>163800</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2015,7 +2015,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="31797360" y="221760"/>
-          <a:ext cx="3782880" cy="3096720"/>
+          <a:ext cx="3782520" cy="3096360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2036,9 +2036,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>298080</xdr:colOff>
+      <xdr:colOff>297720</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2052,7 +2052,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="31746960" y="3351600"/>
-          <a:ext cx="3705840" cy="3018240"/>
+          <a:ext cx="3705480" cy="3017880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2073,9 +2073,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>364320</xdr:colOff>
+      <xdr:colOff>363960</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2089,7 +2089,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="31813200" y="6997320"/>
-          <a:ext cx="3705840" cy="3066840"/>
+          <a:ext cx="3705480" cy="3066480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2115,9 +2115,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>100800</xdr:colOff>
+      <xdr:colOff>100440</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>34920</xdr:rowOff>
+      <xdr:rowOff>34560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2131,7 +2131,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11979000" y="392400"/>
-          <a:ext cx="5190480" cy="3485520"/>
+          <a:ext cx="5190120" cy="3485160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2152,9 +2152,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>29160</xdr:colOff>
+      <xdr:colOff>28800</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>108360</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2168,7 +2168,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="317160" y="392040"/>
-          <a:ext cx="8652600" cy="4610880"/>
+          <a:ext cx="8652240" cy="4610520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2189,9 +2189,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>605520</xdr:colOff>
+      <xdr:colOff>605160</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>91080</xdr:rowOff>
+      <xdr:rowOff>90720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2201,7 +2201,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="871920" y="5799240"/>
-          <a:ext cx="9487080" cy="6372000"/>
+          <a:ext cx="9486720" cy="6371640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2248,9 +2248,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>546120</xdr:colOff>
+      <xdr:colOff>545760</xdr:colOff>
       <xdr:row>110</xdr:row>
-      <xdr:rowOff>136440</xdr:rowOff>
+      <xdr:rowOff>136080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2264,7 +2264,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="812520" y="13030200"/>
-          <a:ext cx="9487080" cy="6372000"/>
+          <a:ext cx="9486720" cy="6371640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2285,9 +2285,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>289080</xdr:colOff>
+      <xdr:colOff>288720</xdr:colOff>
       <xdr:row>154</xdr:row>
-      <xdr:rowOff>77760</xdr:rowOff>
+      <xdr:rowOff>77400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2301,7 +2301,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="812520" y="20683080"/>
-          <a:ext cx="11668320" cy="6372000"/>
+          <a:ext cx="11667960" cy="6371640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2323,7 +2323,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -3329,8 +3329,8 @@
   </sheetPr>
   <dimension ref="A1:K299"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A282" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J304" activeCellId="0" sqref="J304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3414,8 +3414,8 @@
         <v>1</v>
       </c>
       <c r="K2" s="10" t="n">
-        <f aca="false">VLOOKUP(J2,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J2,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3454,8 +3454,8 @@
         <v>3</v>
       </c>
       <c r="K3" s="10" t="n">
-        <f aca="false">VLOOKUP(J3,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J3,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3494,8 +3494,8 @@
         <v>2</v>
       </c>
       <c r="K4" s="10" t="n">
-        <f aca="false">VLOOKUP(J4,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J4,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3534,8 +3534,8 @@
         <v>1</v>
       </c>
       <c r="K5" s="10" t="n">
-        <f aca="false">VLOOKUP(J5,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J5,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3574,8 +3574,8 @@
         <v>1</v>
       </c>
       <c r="K6" s="10" t="n">
-        <f aca="false">VLOOKUP(J6,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J6,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3614,8 +3614,8 @@
         <v>1</v>
       </c>
       <c r="K7" s="10" t="n">
-        <f aca="false">VLOOKUP(J7,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J7,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3654,8 +3654,8 @@
         <v>2</v>
       </c>
       <c r="K8" s="10" t="n">
-        <f aca="false">VLOOKUP(J8,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J8,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3694,8 +3694,8 @@
         <v>3</v>
       </c>
       <c r="K9" s="10" t="n">
-        <f aca="false">VLOOKUP(J9,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J9,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3734,8 +3734,8 @@
         <v>2</v>
       </c>
       <c r="K10" s="10" t="n">
-        <f aca="false">VLOOKUP(J10,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J10,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3774,8 +3774,8 @@
         <v>2</v>
       </c>
       <c r="K11" s="10" t="n">
-        <f aca="false">VLOOKUP(J11,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J11,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3814,8 +3814,8 @@
         <v>3</v>
       </c>
       <c r="K12" s="10" t="n">
-        <f aca="false">VLOOKUP(J12,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J12,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3854,8 +3854,8 @@
         <v>3</v>
       </c>
       <c r="K13" s="10" t="n">
-        <f aca="false">VLOOKUP(J13,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J13,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3894,8 +3894,8 @@
         <v>3</v>
       </c>
       <c r="K14" s="10" t="n">
-        <f aca="false">VLOOKUP(J14,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J14,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3934,8 +3934,8 @@
         <v>2</v>
       </c>
       <c r="K15" s="10" t="n">
-        <f aca="false">VLOOKUP(J15,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J15,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3974,8 +3974,8 @@
         <v>3</v>
       </c>
       <c r="K16" s="10" t="n">
-        <f aca="false">VLOOKUP(J16,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J16,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4014,8 +4014,8 @@
         <v>1</v>
       </c>
       <c r="K17" s="10" t="n">
-        <f aca="false">VLOOKUP(J17,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J17,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4054,8 +4054,8 @@
         <v>2</v>
       </c>
       <c r="K18" s="10" t="n">
-        <f aca="false">VLOOKUP(J18,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J18,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4094,8 +4094,8 @@
         <v>1</v>
       </c>
       <c r="K19" s="10" t="n">
-        <f aca="false">VLOOKUP(J19,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J19,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4134,8 +4134,8 @@
         <v>3</v>
       </c>
       <c r="K20" s="10" t="n">
-        <f aca="false">VLOOKUP(J20,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J20,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4174,8 +4174,8 @@
         <v>1</v>
       </c>
       <c r="K21" s="10" t="n">
-        <f aca="false">VLOOKUP(J21,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J21,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4214,8 +4214,8 @@
         <v>1</v>
       </c>
       <c r="K22" s="10" t="n">
-        <f aca="false">VLOOKUP(J22,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J22,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4254,8 +4254,8 @@
         <v>2</v>
       </c>
       <c r="K23" s="10" t="n">
-        <f aca="false">VLOOKUP(J23,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J23,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4294,8 +4294,8 @@
         <v>2</v>
       </c>
       <c r="K24" s="10" t="n">
-        <f aca="false">VLOOKUP(J24,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J24,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4334,8 +4334,8 @@
         <v>3</v>
       </c>
       <c r="K25" s="10" t="n">
-        <f aca="false">VLOOKUP(J25,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J25,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4374,8 +4374,8 @@
         <v>1</v>
       </c>
       <c r="K26" s="10" t="n">
-        <f aca="false">VLOOKUP(J26,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J26,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4414,8 +4414,8 @@
         <v>2</v>
       </c>
       <c r="K27" s="10" t="n">
-        <f aca="false">VLOOKUP(J27,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J27,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4454,8 +4454,8 @@
         <v>2</v>
       </c>
       <c r="K28" s="10" t="n">
-        <f aca="false">VLOOKUP(J28,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J28,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4494,8 +4494,8 @@
         <v>2</v>
       </c>
       <c r="K29" s="10" t="n">
-        <f aca="false">VLOOKUP(J29,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J29,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4534,8 +4534,8 @@
         <v>2</v>
       </c>
       <c r="K30" s="10" t="n">
-        <f aca="false">VLOOKUP(J30,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J30,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4574,8 +4574,8 @@
         <v>1</v>
       </c>
       <c r="K31" s="10" t="n">
-        <f aca="false">VLOOKUP(J31,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J31,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4614,8 +4614,8 @@
         <v>3</v>
       </c>
       <c r="K32" s="10" t="n">
-        <f aca="false">VLOOKUP(J32,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J32,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4654,8 +4654,8 @@
         <v>3</v>
       </c>
       <c r="K33" s="10" t="n">
-        <f aca="false">VLOOKUP(J33,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J33,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4694,8 +4694,8 @@
         <v>1</v>
       </c>
       <c r="K34" s="10" t="n">
-        <f aca="false">VLOOKUP(J34,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J34,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4734,8 +4734,8 @@
         <v>1</v>
       </c>
       <c r="K35" s="10" t="n">
-        <f aca="false">VLOOKUP(J35,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J35,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4774,8 +4774,8 @@
         <v>1</v>
       </c>
       <c r="K36" s="10" t="n">
-        <f aca="false">VLOOKUP(J36,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J36,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4814,8 +4814,8 @@
         <v>1</v>
       </c>
       <c r="K37" s="10" t="n">
-        <f aca="false">VLOOKUP(J37,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J37,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4854,8 +4854,8 @@
         <v>2</v>
       </c>
       <c r="K38" s="10" t="n">
-        <f aca="false">VLOOKUP(J38,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J38,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4894,8 +4894,8 @@
         <v>1</v>
       </c>
       <c r="K39" s="10" t="n">
-        <f aca="false">VLOOKUP(J39,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J39,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4934,8 +4934,8 @@
         <v>2</v>
       </c>
       <c r="K40" s="10" t="n">
-        <f aca="false">VLOOKUP(J40,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J40,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4974,8 +4974,8 @@
         <v>1</v>
       </c>
       <c r="K41" s="10" t="n">
-        <f aca="false">VLOOKUP(J41,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J41,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5014,8 +5014,8 @@
         <v>1</v>
       </c>
       <c r="K42" s="10" t="n">
-        <f aca="false">VLOOKUP(J42,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J42,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5054,8 +5054,8 @@
         <v>3</v>
       </c>
       <c r="K43" s="10" t="n">
-        <f aca="false">VLOOKUP(J43,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J43,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5094,8 +5094,8 @@
         <v>3</v>
       </c>
       <c r="K44" s="10" t="n">
-        <f aca="false">VLOOKUP(J44,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J44,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5134,8 +5134,8 @@
         <v>1</v>
       </c>
       <c r="K45" s="10" t="n">
-        <f aca="false">VLOOKUP(J45,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J45,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5174,8 +5174,8 @@
         <v>1</v>
       </c>
       <c r="K46" s="10" t="n">
-        <f aca="false">VLOOKUP(J46,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J46,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5214,8 +5214,8 @@
         <v>1</v>
       </c>
       <c r="K47" s="10" t="n">
-        <f aca="false">VLOOKUP(J47,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J47,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5254,8 +5254,8 @@
         <v>3</v>
       </c>
       <c r="K48" s="10" t="n">
-        <f aca="false">VLOOKUP(J48,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J48,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5294,8 +5294,8 @@
         <v>3</v>
       </c>
       <c r="K49" s="10" t="n">
-        <f aca="false">VLOOKUP(J49,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J49,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5334,8 +5334,8 @@
         <v>3</v>
       </c>
       <c r="K50" s="10" t="n">
-        <f aca="false">VLOOKUP(J50,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J50,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5374,8 +5374,8 @@
         <v>3</v>
       </c>
       <c r="K51" s="10" t="n">
-        <f aca="false">VLOOKUP(J51,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J51,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5414,8 +5414,8 @@
         <v>1</v>
       </c>
       <c r="K52" s="10" t="n">
-        <f aca="false">VLOOKUP(J52,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J52,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5454,8 +5454,8 @@
         <v>3</v>
       </c>
       <c r="K53" s="10" t="n">
-        <f aca="false">VLOOKUP(J53,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J53,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5494,8 +5494,8 @@
         <v>1</v>
       </c>
       <c r="K54" s="10" t="n">
-        <f aca="false">VLOOKUP(J54,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J54,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5534,8 +5534,8 @@
         <v>3</v>
       </c>
       <c r="K55" s="10" t="n">
-        <f aca="false">VLOOKUP(J55,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J55,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5574,8 +5574,8 @@
         <v>1</v>
       </c>
       <c r="K56" s="10" t="n">
-        <f aca="false">VLOOKUP(J56,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J56,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5614,8 +5614,8 @@
         <v>1</v>
       </c>
       <c r="K57" s="10" t="n">
-        <f aca="false">VLOOKUP(J57,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J57,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5654,8 +5654,8 @@
         <v>2</v>
       </c>
       <c r="K58" s="10" t="n">
-        <f aca="false">VLOOKUP(J58,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J58,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5694,8 +5694,8 @@
         <v>3</v>
       </c>
       <c r="K59" s="10" t="n">
-        <f aca="false">VLOOKUP(J59,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J59,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5734,8 +5734,8 @@
         <v>3</v>
       </c>
       <c r="K60" s="10" t="n">
-        <f aca="false">VLOOKUP(J60,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J60,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5774,8 +5774,8 @@
         <v>1</v>
       </c>
       <c r="K61" s="10" t="n">
-        <f aca="false">VLOOKUP(J61,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J61,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5814,8 +5814,8 @@
         <v>2</v>
       </c>
       <c r="K62" s="10" t="n">
-        <f aca="false">VLOOKUP(J62,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J62,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5854,8 +5854,8 @@
         <v>1</v>
       </c>
       <c r="K63" s="10" t="n">
-        <f aca="false">VLOOKUP(J63,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J63,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5894,8 +5894,8 @@
         <v>1</v>
       </c>
       <c r="K64" s="10" t="n">
-        <f aca="false">VLOOKUP(J64,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J64,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5934,8 +5934,8 @@
         <v>3</v>
       </c>
       <c r="K65" s="10" t="n">
-        <f aca="false">VLOOKUP(J65,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J65,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5974,8 +5974,8 @@
         <v>1</v>
       </c>
       <c r="K66" s="10" t="n">
-        <f aca="false">VLOOKUP(J66,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J66,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6014,8 +6014,8 @@
         <v>1</v>
       </c>
       <c r="K67" s="10" t="n">
-        <f aca="false">VLOOKUP(J67,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J67,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6054,8 +6054,8 @@
         <v>3</v>
       </c>
       <c r="K68" s="10" t="n">
-        <f aca="false">VLOOKUP(J68,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J68,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6094,8 +6094,8 @@
         <v>3</v>
       </c>
       <c r="K69" s="10" t="n">
-        <f aca="false">VLOOKUP(J69,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J69,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6134,8 +6134,8 @@
         <v>1</v>
       </c>
       <c r="K70" s="10" t="n">
-        <f aca="false">VLOOKUP(J70,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J70,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6174,8 +6174,8 @@
         <v>3</v>
       </c>
       <c r="K71" s="10" t="n">
-        <f aca="false">VLOOKUP(J71,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J71,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6214,8 +6214,8 @@
         <v>1</v>
       </c>
       <c r="K72" s="10" t="n">
-        <f aca="false">VLOOKUP(J72,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J72,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6254,8 +6254,8 @@
         <v>2</v>
       </c>
       <c r="K73" s="10" t="n">
-        <f aca="false">VLOOKUP(J73,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J73,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6294,8 +6294,8 @@
         <v>3</v>
       </c>
       <c r="K74" s="10" t="n">
-        <f aca="false">VLOOKUP(J74,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J74,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6334,8 +6334,8 @@
         <v>3</v>
       </c>
       <c r="K75" s="10" t="n">
-        <f aca="false">VLOOKUP(J75,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J75,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6374,8 +6374,8 @@
         <v>3</v>
       </c>
       <c r="K76" s="10" t="n">
-        <f aca="false">VLOOKUP(J76,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J76,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6414,8 +6414,8 @@
         <v>3</v>
       </c>
       <c r="K77" s="10" t="n">
-        <f aca="false">VLOOKUP(J77,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J77,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6454,8 +6454,8 @@
         <v>2</v>
       </c>
       <c r="K78" s="10" t="n">
-        <f aca="false">VLOOKUP(J78,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J78,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6494,8 +6494,8 @@
         <v>1</v>
       </c>
       <c r="K79" s="10" t="n">
-        <f aca="false">VLOOKUP(J79,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J79,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6534,8 +6534,8 @@
         <v>3</v>
       </c>
       <c r="K80" s="10" t="n">
-        <f aca="false">VLOOKUP(J80,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J80,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6574,8 +6574,8 @@
         <v>1</v>
       </c>
       <c r="K81" s="10" t="n">
-        <f aca="false">VLOOKUP(J81,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J81,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6614,8 +6614,8 @@
         <v>2</v>
       </c>
       <c r="K82" s="10" t="n">
-        <f aca="false">VLOOKUP(J82,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J82,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6654,8 +6654,8 @@
         <v>2</v>
       </c>
       <c r="K83" s="10" t="n">
-        <f aca="false">VLOOKUP(J83,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J83,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6694,8 +6694,8 @@
         <v>2</v>
       </c>
       <c r="K84" s="10" t="n">
-        <f aca="false">VLOOKUP(J84,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J84,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6734,8 +6734,8 @@
         <v>2</v>
       </c>
       <c r="K85" s="10" t="n">
-        <f aca="false">VLOOKUP(J85,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J85,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6774,8 +6774,8 @@
         <v>1</v>
       </c>
       <c r="K86" s="10" t="n">
-        <f aca="false">VLOOKUP(J86,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J86,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6814,8 +6814,8 @@
         <v>2</v>
       </c>
       <c r="K87" s="10" t="n">
-        <f aca="false">VLOOKUP(J87,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J87,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6854,8 +6854,8 @@
         <v>1</v>
       </c>
       <c r="K88" s="10" t="n">
-        <f aca="false">VLOOKUP(J88,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J88,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6894,8 +6894,8 @@
         <v>3</v>
       </c>
       <c r="K89" s="10" t="n">
-        <f aca="false">VLOOKUP(J89,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J89,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6934,8 +6934,8 @@
         <v>1</v>
       </c>
       <c r="K90" s="10" t="n">
-        <f aca="false">VLOOKUP(J90,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J90,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6974,8 +6974,8 @@
         <v>3</v>
       </c>
       <c r="K91" s="10" t="n">
-        <f aca="false">VLOOKUP(J91,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J91,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7014,8 +7014,8 @@
         <v>3</v>
       </c>
       <c r="K92" s="10" t="n">
-        <f aca="false">VLOOKUP(J92,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J92,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7054,8 +7054,8 @@
         <v>1</v>
       </c>
       <c r="K93" s="10" t="n">
-        <f aca="false">VLOOKUP(J93,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J93,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7094,8 +7094,8 @@
         <v>2</v>
       </c>
       <c r="K94" s="10" t="n">
-        <f aca="false">VLOOKUP(J94,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J94,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7134,8 +7134,8 @@
         <v>3</v>
       </c>
       <c r="K95" s="10" t="n">
-        <f aca="false">VLOOKUP(J95,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J95,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7174,8 +7174,8 @@
         <v>2</v>
       </c>
       <c r="K96" s="10" t="n">
-        <f aca="false">VLOOKUP(J96,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J96,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7214,8 +7214,8 @@
         <v>2</v>
       </c>
       <c r="K97" s="10" t="n">
-        <f aca="false">VLOOKUP(J97,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J97,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7254,8 +7254,8 @@
         <v>2</v>
       </c>
       <c r="K98" s="10" t="n">
-        <f aca="false">VLOOKUP(J98,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J98,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7294,8 +7294,8 @@
         <v>3</v>
       </c>
       <c r="K99" s="10" t="n">
-        <f aca="false">VLOOKUP(J99,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J99,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7334,8 +7334,8 @@
         <v>3</v>
       </c>
       <c r="K100" s="10" t="n">
-        <f aca="false">VLOOKUP(J100,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J100,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7374,8 +7374,8 @@
         <v>3</v>
       </c>
       <c r="K101" s="10" t="n">
-        <f aca="false">VLOOKUP(J101,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J101,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7414,8 +7414,8 @@
         <v>3</v>
       </c>
       <c r="K102" s="10" t="n">
-        <f aca="false">VLOOKUP(J102,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J102,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7454,8 +7454,8 @@
         <v>1</v>
       </c>
       <c r="K103" s="10" t="n">
-        <f aca="false">VLOOKUP(J103,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J103,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7494,8 +7494,8 @@
         <v>3</v>
       </c>
       <c r="K104" s="10" t="n">
-        <f aca="false">VLOOKUP(J104,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J104,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7534,8 +7534,8 @@
         <v>2</v>
       </c>
       <c r="K105" s="10" t="n">
-        <f aca="false">VLOOKUP(J105,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J105,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7574,8 +7574,8 @@
         <v>3</v>
       </c>
       <c r="K106" s="10" t="n">
-        <f aca="false">VLOOKUP(J106,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J106,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7614,8 +7614,8 @@
         <v>3</v>
       </c>
       <c r="K107" s="10" t="n">
-        <f aca="false">VLOOKUP(J107,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J107,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7654,8 +7654,8 @@
         <v>3</v>
       </c>
       <c r="K108" s="10" t="n">
-        <f aca="false">VLOOKUP(J108,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J108,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7694,8 +7694,8 @@
         <v>2</v>
       </c>
       <c r="K109" s="10" t="n">
-        <f aca="false">VLOOKUP(J109,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J109,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7734,8 +7734,8 @@
         <v>3</v>
       </c>
       <c r="K110" s="10" t="n">
-        <f aca="false">VLOOKUP(J110,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J110,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7774,8 +7774,8 @@
         <v>1</v>
       </c>
       <c r="K111" s="10" t="n">
-        <f aca="false">VLOOKUP(J111,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J111,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7814,8 +7814,8 @@
         <v>1</v>
       </c>
       <c r="K112" s="10" t="n">
-        <f aca="false">VLOOKUP(J112,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J112,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7854,8 +7854,8 @@
         <v>1</v>
       </c>
       <c r="K113" s="10" t="n">
-        <f aca="false">VLOOKUP(J113,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J113,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7894,8 +7894,8 @@
         <v>3</v>
       </c>
       <c r="K114" s="10" t="n">
-        <f aca="false">VLOOKUP(J114,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J114,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7934,8 +7934,8 @@
         <v>1</v>
       </c>
       <c r="K115" s="10" t="n">
-        <f aca="false">VLOOKUP(J115,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J115,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7974,8 +7974,8 @@
         <v>1</v>
       </c>
       <c r="K116" s="10" t="n">
-        <f aca="false">VLOOKUP(J116,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J116,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8014,8 +8014,8 @@
         <v>1</v>
       </c>
       <c r="K117" s="10" t="n">
-        <f aca="false">VLOOKUP(J117,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J117,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8054,8 +8054,8 @@
         <v>3</v>
       </c>
       <c r="K118" s="10" t="n">
-        <f aca="false">VLOOKUP(J118,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J118,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8094,8 +8094,8 @@
         <v>3</v>
       </c>
       <c r="K119" s="10" t="n">
-        <f aca="false">VLOOKUP(J119,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J119,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8134,8 +8134,8 @@
         <v>2</v>
       </c>
       <c r="K120" s="10" t="n">
-        <f aca="false">VLOOKUP(J120,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J120,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8174,8 +8174,8 @@
         <v>2</v>
       </c>
       <c r="K121" s="10" t="n">
-        <f aca="false">VLOOKUP(J121,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J121,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8214,8 +8214,8 @@
         <v>2</v>
       </c>
       <c r="K122" s="10" t="n">
-        <f aca="false">VLOOKUP(J122,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J122,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8254,8 +8254,8 @@
         <v>3</v>
       </c>
       <c r="K123" s="10" t="n">
-        <f aca="false">VLOOKUP(J123,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J123,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8294,8 +8294,8 @@
         <v>3</v>
       </c>
       <c r="K124" s="10" t="n">
-        <f aca="false">VLOOKUP(J124,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J124,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8334,8 +8334,8 @@
         <v>1</v>
       </c>
       <c r="K125" s="10" t="n">
-        <f aca="false">VLOOKUP(J125,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J125,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8374,8 +8374,8 @@
         <v>3</v>
       </c>
       <c r="K126" s="10" t="n">
-        <f aca="false">VLOOKUP(J126,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J126,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8414,8 +8414,8 @@
         <v>1</v>
       </c>
       <c r="K127" s="10" t="n">
-        <f aca="false">VLOOKUP(J127,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J127,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8454,8 +8454,8 @@
         <v>2</v>
       </c>
       <c r="K128" s="10" t="n">
-        <f aca="false">VLOOKUP(J128,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J128,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8494,8 +8494,8 @@
         <v>2</v>
       </c>
       <c r="K129" s="10" t="n">
-        <f aca="false">VLOOKUP(J129,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J129,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8534,8 +8534,8 @@
         <v>1</v>
       </c>
       <c r="K130" s="10" t="n">
-        <f aca="false">VLOOKUP(J130,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J130,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8574,8 +8574,8 @@
         <v>3</v>
       </c>
       <c r="K131" s="10" t="n">
-        <f aca="false">VLOOKUP(J131,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J131,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8614,8 +8614,8 @@
         <v>3</v>
       </c>
       <c r="K132" s="10" t="n">
-        <f aca="false">VLOOKUP(J132,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J132,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8654,8 +8654,8 @@
         <v>1</v>
       </c>
       <c r="K133" s="10" t="n">
-        <f aca="false">VLOOKUP(J133,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J133,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8694,8 +8694,8 @@
         <v>3</v>
       </c>
       <c r="K134" s="10" t="n">
-        <f aca="false">VLOOKUP(J134,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J134,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8734,8 +8734,8 @@
         <v>1</v>
       </c>
       <c r="K135" s="10" t="n">
-        <f aca="false">VLOOKUP(J135,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J135,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8774,8 +8774,8 @@
         <v>2</v>
       </c>
       <c r="K136" s="10" t="n">
-        <f aca="false">VLOOKUP(J136,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J136,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8814,8 +8814,8 @@
         <v>2</v>
       </c>
       <c r="K137" s="10" t="n">
-        <f aca="false">VLOOKUP(J137,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J137,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8854,8 +8854,8 @@
         <v>3</v>
       </c>
       <c r="K138" s="10" t="n">
-        <f aca="false">VLOOKUP(J138,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J138,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8894,8 +8894,8 @@
         <v>3</v>
       </c>
       <c r="K139" s="10" t="n">
-        <f aca="false">VLOOKUP(J139,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J139,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8934,8 +8934,8 @@
         <v>2</v>
       </c>
       <c r="K140" s="10" t="n">
-        <f aca="false">VLOOKUP(J140,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J140,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8974,8 +8974,8 @@
         <v>1</v>
       </c>
       <c r="K141" s="10" t="n">
-        <f aca="false">VLOOKUP(J141,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J141,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9014,8 +9014,8 @@
         <v>3</v>
       </c>
       <c r="K142" s="10" t="n">
-        <f aca="false">VLOOKUP(J142,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J142,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9054,8 +9054,8 @@
         <v>1</v>
       </c>
       <c r="K143" s="10" t="n">
-        <f aca="false">VLOOKUP(J143,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J143,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9094,8 +9094,8 @@
         <v>2</v>
       </c>
       <c r="K144" s="10" t="n">
-        <f aca="false">VLOOKUP(J144,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J144,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9134,8 +9134,8 @@
         <v>2</v>
       </c>
       <c r="K145" s="10" t="n">
-        <f aca="false">VLOOKUP(J145,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J145,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9174,8 +9174,8 @@
         <v>3</v>
       </c>
       <c r="K146" s="10" t="n">
-        <f aca="false">VLOOKUP(J146,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J146,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9214,8 +9214,8 @@
         <v>2</v>
       </c>
       <c r="K147" s="10" t="n">
-        <f aca="false">VLOOKUP(J147,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J147,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9254,8 +9254,8 @@
         <v>1</v>
       </c>
       <c r="K148" s="10" t="n">
-        <f aca="false">VLOOKUP(J148,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J148,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9294,8 +9294,8 @@
         <v>1</v>
       </c>
       <c r="K149" s="10" t="n">
-        <f aca="false">VLOOKUP(J149,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J149,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9334,8 +9334,8 @@
         <v>2</v>
       </c>
       <c r="K150" s="10" t="n">
-        <f aca="false">VLOOKUP(J150,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J150,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9374,8 +9374,8 @@
         <v>3</v>
       </c>
       <c r="K151" s="10" t="n">
-        <f aca="false">VLOOKUP(J151,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J151,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9414,8 +9414,8 @@
         <v>2</v>
       </c>
       <c r="K152" s="10" t="n">
-        <f aca="false">VLOOKUP(J152,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J152,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9454,8 +9454,8 @@
         <v>2</v>
       </c>
       <c r="K153" s="10" t="n">
-        <f aca="false">VLOOKUP(J153,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J153,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9494,8 +9494,8 @@
         <v>3</v>
       </c>
       <c r="K154" s="10" t="n">
-        <f aca="false">VLOOKUP(J154,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J154,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9534,8 +9534,8 @@
         <v>3</v>
       </c>
       <c r="K155" s="10" t="n">
-        <f aca="false">VLOOKUP(J155,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J155,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9574,8 +9574,8 @@
         <v>1</v>
       </c>
       <c r="K156" s="10" t="n">
-        <f aca="false">VLOOKUP(J156,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J156,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9614,8 +9614,8 @@
         <v>3</v>
       </c>
       <c r="K157" s="10" t="n">
-        <f aca="false">VLOOKUP(J157,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J157,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9654,7 +9654,7 @@
         <v>183</v>
       </c>
       <c r="K158" s="10" t="e">
-        <f aca="false">VLOOKUP(J158,Summary!$B$3:$G$5,5,0)</f>
+        <f aca="false">VLOOKUP(J158,Summary!$B$3:$G$5,6,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9694,8 +9694,8 @@
         <v>3</v>
       </c>
       <c r="K159" s="10" t="n">
-        <f aca="false">VLOOKUP(J159,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J159,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9734,8 +9734,8 @@
         <v>3</v>
       </c>
       <c r="K160" s="10" t="n">
-        <f aca="false">VLOOKUP(J160,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J160,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9774,8 +9774,8 @@
         <v>2</v>
       </c>
       <c r="K161" s="10" t="n">
-        <f aca="false">VLOOKUP(J161,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J161,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9814,8 +9814,8 @@
         <v>3</v>
       </c>
       <c r="K162" s="10" t="n">
-        <f aca="false">VLOOKUP(J162,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J162,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9854,8 +9854,8 @@
         <v>2</v>
       </c>
       <c r="K163" s="10" t="n">
-        <f aca="false">VLOOKUP(J163,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J163,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9894,8 +9894,8 @@
         <v>1</v>
       </c>
       <c r="K164" s="10" t="n">
-        <f aca="false">VLOOKUP(J164,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J164,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9934,8 +9934,8 @@
         <v>3</v>
       </c>
       <c r="K165" s="10" t="n">
-        <f aca="false">VLOOKUP(J165,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J165,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9974,8 +9974,8 @@
         <v>2</v>
       </c>
       <c r="K166" s="10" t="n">
-        <f aca="false">VLOOKUP(J166,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J166,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10014,8 +10014,8 @@
         <v>3</v>
       </c>
       <c r="K167" s="10" t="n">
-        <f aca="false">VLOOKUP(J167,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J167,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10054,8 +10054,8 @@
         <v>3</v>
       </c>
       <c r="K168" s="10" t="n">
-        <f aca="false">VLOOKUP(J168,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J168,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10094,8 +10094,8 @@
         <v>3</v>
       </c>
       <c r="K169" s="10" t="n">
-        <f aca="false">VLOOKUP(J169,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J169,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10134,8 +10134,8 @@
         <v>3</v>
       </c>
       <c r="K170" s="10" t="n">
-        <f aca="false">VLOOKUP(J170,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J170,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10174,8 +10174,8 @@
         <v>3</v>
       </c>
       <c r="K171" s="10" t="n">
-        <f aca="false">VLOOKUP(J171,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J171,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10214,8 +10214,8 @@
         <v>2</v>
       </c>
       <c r="K172" s="10" t="n">
-        <f aca="false">VLOOKUP(J172,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J172,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10254,8 +10254,8 @@
         <v>1</v>
       </c>
       <c r="K173" s="10" t="n">
-        <f aca="false">VLOOKUP(J173,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J173,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10294,8 +10294,8 @@
         <v>2</v>
       </c>
       <c r="K174" s="10" t="n">
-        <f aca="false">VLOOKUP(J174,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J174,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10334,8 +10334,8 @@
         <v>3</v>
       </c>
       <c r="K175" s="10" t="n">
-        <f aca="false">VLOOKUP(J175,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J175,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10374,8 +10374,8 @@
         <v>1</v>
       </c>
       <c r="K176" s="10" t="n">
-        <f aca="false">VLOOKUP(J176,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J176,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10414,8 +10414,8 @@
         <v>1</v>
       </c>
       <c r="K177" s="10" t="n">
-        <f aca="false">VLOOKUP(J177,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J177,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10454,8 +10454,8 @@
         <v>3</v>
       </c>
       <c r="K178" s="10" t="n">
-        <f aca="false">VLOOKUP(J178,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J178,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10494,8 +10494,8 @@
         <v>2</v>
       </c>
       <c r="K179" s="10" t="n">
-        <f aca="false">VLOOKUP(J179,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J179,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10534,8 +10534,8 @@
         <v>3</v>
       </c>
       <c r="K180" s="10" t="n">
-        <f aca="false">VLOOKUP(J180,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J180,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10574,8 +10574,8 @@
         <v>2</v>
       </c>
       <c r="K181" s="10" t="n">
-        <f aca="false">VLOOKUP(J181,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J181,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10614,8 +10614,8 @@
         <v>3</v>
       </c>
       <c r="K182" s="10" t="n">
-        <f aca="false">VLOOKUP(J182,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J182,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10654,8 +10654,8 @@
         <v>2</v>
       </c>
       <c r="K183" s="10" t="n">
-        <f aca="false">VLOOKUP(J183,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J183,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10694,8 +10694,8 @@
         <v>2</v>
       </c>
       <c r="K184" s="10" t="n">
-        <f aca="false">VLOOKUP(J184,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J184,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10734,8 +10734,8 @@
         <v>3</v>
       </c>
       <c r="K185" s="10" t="n">
-        <f aca="false">VLOOKUP(J185,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J185,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10774,8 +10774,8 @@
         <v>3</v>
       </c>
       <c r="K186" s="10" t="n">
-        <f aca="false">VLOOKUP(J186,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J186,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10814,8 +10814,8 @@
         <v>3</v>
       </c>
       <c r="K187" s="10" t="n">
-        <f aca="false">VLOOKUP(J187,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J187,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10854,8 +10854,8 @@
         <v>3</v>
       </c>
       <c r="K188" s="10" t="n">
-        <f aca="false">VLOOKUP(J188,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J188,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10894,8 +10894,8 @@
         <v>3</v>
       </c>
       <c r="K189" s="10" t="n">
-        <f aca="false">VLOOKUP(J189,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J189,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10934,8 +10934,8 @@
         <v>3</v>
       </c>
       <c r="K190" s="10" t="n">
-        <f aca="false">VLOOKUP(J190,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J190,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10974,8 +10974,8 @@
         <v>3</v>
       </c>
       <c r="K191" s="10" t="n">
-        <f aca="false">VLOOKUP(J191,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J191,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11014,8 +11014,8 @@
         <v>1</v>
       </c>
       <c r="K192" s="10" t="n">
-        <f aca="false">VLOOKUP(J192,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J192,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11054,8 +11054,8 @@
         <v>2</v>
       </c>
       <c r="K193" s="10" t="n">
-        <f aca="false">VLOOKUP(J193,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J193,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11094,8 +11094,8 @@
         <v>2</v>
       </c>
       <c r="K194" s="10" t="n">
-        <f aca="false">VLOOKUP(J194,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J194,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11134,8 +11134,8 @@
         <v>1</v>
       </c>
       <c r="K195" s="10" t="n">
-        <f aca="false">VLOOKUP(J195,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J195,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11174,8 +11174,8 @@
         <v>1</v>
       </c>
       <c r="K196" s="10" t="n">
-        <f aca="false">VLOOKUP(J196,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J196,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11214,8 +11214,8 @@
         <v>3</v>
       </c>
       <c r="K197" s="10" t="n">
-        <f aca="false">VLOOKUP(J197,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J197,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11254,8 +11254,8 @@
         <v>2</v>
       </c>
       <c r="K198" s="10" t="n">
-        <f aca="false">VLOOKUP(J198,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J198,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11294,8 +11294,8 @@
         <v>3</v>
       </c>
       <c r="K199" s="10" t="n">
-        <f aca="false">VLOOKUP(J199,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J199,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11334,8 +11334,8 @@
         <v>1</v>
       </c>
       <c r="K200" s="10" t="n">
-        <f aca="false">VLOOKUP(J200,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J200,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11374,8 +11374,8 @@
         <v>3</v>
       </c>
       <c r="K201" s="10" t="n">
-        <f aca="false">VLOOKUP(J201,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J201,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11414,8 +11414,8 @@
         <v>1</v>
       </c>
       <c r="K202" s="10" t="n">
-        <f aca="false">VLOOKUP(J202,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J202,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11454,8 +11454,8 @@
         <v>1</v>
       </c>
       <c r="K203" s="10" t="n">
-        <f aca="false">VLOOKUP(J203,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J203,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11494,8 +11494,8 @@
         <v>1</v>
       </c>
       <c r="K204" s="10" t="n">
-        <f aca="false">VLOOKUP(J204,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J204,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11534,8 +11534,8 @@
         <v>1</v>
       </c>
       <c r="K205" s="10" t="n">
-        <f aca="false">VLOOKUP(J205,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J205,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11574,8 +11574,8 @@
         <v>3</v>
       </c>
       <c r="K206" s="10" t="n">
-        <f aca="false">VLOOKUP(J206,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J206,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11614,8 +11614,8 @@
         <v>3</v>
       </c>
       <c r="K207" s="10" t="n">
-        <f aca="false">VLOOKUP(J207,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J207,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11654,8 +11654,8 @@
         <v>2</v>
       </c>
       <c r="K208" s="10" t="n">
-        <f aca="false">VLOOKUP(J208,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J208,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11694,8 +11694,8 @@
         <v>2</v>
       </c>
       <c r="K209" s="10" t="n">
-        <f aca="false">VLOOKUP(J209,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J209,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11734,8 +11734,8 @@
         <v>3</v>
       </c>
       <c r="K210" s="10" t="n">
-        <f aca="false">VLOOKUP(J210,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J210,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11774,8 +11774,8 @@
         <v>2</v>
       </c>
       <c r="K211" s="10" t="n">
-        <f aca="false">VLOOKUP(J211,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J211,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11814,8 +11814,8 @@
         <v>1</v>
       </c>
       <c r="K212" s="10" t="n">
-        <f aca="false">VLOOKUP(J212,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J212,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11854,8 +11854,8 @@
         <v>1</v>
       </c>
       <c r="K213" s="10" t="n">
-        <f aca="false">VLOOKUP(J213,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J213,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11894,7 +11894,7 @@
         <v>183</v>
       </c>
       <c r="K214" s="10" t="e">
-        <f aca="false">VLOOKUP(J214,Summary!$B$3:$G$5,5,0)</f>
+        <f aca="false">VLOOKUP(J214,Summary!$B$3:$G$5,6,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -11934,8 +11934,8 @@
         <v>3</v>
       </c>
       <c r="K215" s="10" t="n">
-        <f aca="false">VLOOKUP(J215,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J215,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11974,8 +11974,8 @@
         <v>2</v>
       </c>
       <c r="K216" s="10" t="n">
-        <f aca="false">VLOOKUP(J216,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J216,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12014,8 +12014,8 @@
         <v>3</v>
       </c>
       <c r="K217" s="10" t="n">
-        <f aca="false">VLOOKUP(J217,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J217,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12054,8 +12054,8 @@
         <v>2</v>
       </c>
       <c r="K218" s="10" t="n">
-        <f aca="false">VLOOKUP(J218,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J218,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12094,8 +12094,8 @@
         <v>1</v>
       </c>
       <c r="K219" s="10" t="n">
-        <f aca="false">VLOOKUP(J219,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J219,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12134,8 +12134,8 @@
         <v>3</v>
       </c>
       <c r="K220" s="10" t="n">
-        <f aca="false">VLOOKUP(J220,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J220,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12174,8 +12174,8 @@
         <v>1</v>
       </c>
       <c r="K221" s="10" t="n">
-        <f aca="false">VLOOKUP(J221,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J221,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12214,8 +12214,8 @@
         <v>3</v>
       </c>
       <c r="K222" s="10" t="n">
-        <f aca="false">VLOOKUP(J222,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J222,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12254,8 +12254,8 @@
         <v>2</v>
       </c>
       <c r="K223" s="10" t="n">
-        <f aca="false">VLOOKUP(J223,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J223,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12294,8 +12294,8 @@
         <v>2</v>
       </c>
       <c r="K224" s="10" t="n">
-        <f aca="false">VLOOKUP(J224,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J224,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12334,8 +12334,8 @@
         <v>2</v>
       </c>
       <c r="K225" s="10" t="n">
-        <f aca="false">VLOOKUP(J225,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J225,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12374,8 +12374,8 @@
         <v>3</v>
       </c>
       <c r="K226" s="10" t="n">
-        <f aca="false">VLOOKUP(J226,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J226,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12414,8 +12414,8 @@
         <v>2</v>
       </c>
       <c r="K227" s="10" t="n">
-        <f aca="false">VLOOKUP(J227,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J227,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12454,8 +12454,8 @@
         <v>2</v>
       </c>
       <c r="K228" s="10" t="n">
-        <f aca="false">VLOOKUP(J228,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J228,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12494,8 +12494,8 @@
         <v>3</v>
       </c>
       <c r="K229" s="10" t="n">
-        <f aca="false">VLOOKUP(J229,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J229,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12534,8 +12534,8 @@
         <v>2</v>
       </c>
       <c r="K230" s="10" t="n">
-        <f aca="false">VLOOKUP(J230,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J230,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12574,8 +12574,8 @@
         <v>3</v>
       </c>
       <c r="K231" s="10" t="n">
-        <f aca="false">VLOOKUP(J231,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J231,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12614,8 +12614,8 @@
         <v>1</v>
       </c>
       <c r="K232" s="10" t="n">
-        <f aca="false">VLOOKUP(J232,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J232,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12654,8 +12654,8 @@
         <v>3</v>
       </c>
       <c r="K233" s="10" t="n">
-        <f aca="false">VLOOKUP(J233,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J233,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12694,8 +12694,8 @@
         <v>2</v>
       </c>
       <c r="K234" s="10" t="n">
-        <f aca="false">VLOOKUP(J234,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J234,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12734,8 +12734,8 @@
         <v>1</v>
       </c>
       <c r="K235" s="10" t="n">
-        <f aca="false">VLOOKUP(J235,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J235,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12774,8 +12774,8 @@
         <v>3</v>
       </c>
       <c r="K236" s="10" t="n">
-        <f aca="false">VLOOKUP(J236,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J236,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12814,8 +12814,8 @@
         <v>2</v>
       </c>
       <c r="K237" s="10" t="n">
-        <f aca="false">VLOOKUP(J237,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J237,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12854,8 +12854,8 @@
         <v>3</v>
       </c>
       <c r="K238" s="10" t="n">
-        <f aca="false">VLOOKUP(J238,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J238,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12894,8 +12894,8 @@
         <v>3</v>
       </c>
       <c r="K239" s="10" t="n">
-        <f aca="false">VLOOKUP(J239,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J239,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12934,8 +12934,8 @@
         <v>3</v>
       </c>
       <c r="K240" s="10" t="n">
-        <f aca="false">VLOOKUP(J240,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J240,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12974,8 +12974,8 @@
         <v>2</v>
       </c>
       <c r="K241" s="10" t="n">
-        <f aca="false">VLOOKUP(J241,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J241,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13014,8 +13014,8 @@
         <v>2</v>
       </c>
       <c r="K242" s="10" t="n">
-        <f aca="false">VLOOKUP(J242,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J242,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13054,8 +13054,8 @@
         <v>3</v>
       </c>
       <c r="K243" s="10" t="n">
-        <f aca="false">VLOOKUP(J243,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J243,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13094,8 +13094,8 @@
         <v>3</v>
       </c>
       <c r="K244" s="10" t="n">
-        <f aca="false">VLOOKUP(J244,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J244,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13134,8 +13134,8 @@
         <v>1</v>
       </c>
       <c r="K245" s="10" t="n">
-        <f aca="false">VLOOKUP(J245,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J245,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13174,8 +13174,8 @@
         <v>1</v>
       </c>
       <c r="K246" s="10" t="n">
-        <f aca="false">VLOOKUP(J246,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J246,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13214,8 +13214,8 @@
         <v>1</v>
       </c>
       <c r="K247" s="10" t="n">
-        <f aca="false">VLOOKUP(J247,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J247,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13254,8 +13254,8 @@
         <v>3</v>
       </c>
       <c r="K248" s="10" t="n">
-        <f aca="false">VLOOKUP(J248,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J248,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13294,8 +13294,8 @@
         <v>2</v>
       </c>
       <c r="K249" s="10" t="n">
-        <f aca="false">VLOOKUP(J249,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J249,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13334,8 +13334,8 @@
         <v>2</v>
       </c>
       <c r="K250" s="10" t="n">
-        <f aca="false">VLOOKUP(J250,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J250,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13374,8 +13374,8 @@
         <v>3</v>
       </c>
       <c r="K251" s="10" t="n">
-        <f aca="false">VLOOKUP(J251,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J251,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13414,8 +13414,8 @@
         <v>3</v>
       </c>
       <c r="K252" s="10" t="n">
-        <f aca="false">VLOOKUP(J252,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J252,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13454,8 +13454,8 @@
         <v>2</v>
       </c>
       <c r="K253" s="10" t="n">
-        <f aca="false">VLOOKUP(J253,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J253,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13494,8 +13494,8 @@
         <v>3</v>
       </c>
       <c r="K254" s="10" t="n">
-        <f aca="false">VLOOKUP(J254,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J254,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13534,8 +13534,8 @@
         <v>3</v>
       </c>
       <c r="K255" s="10" t="n">
-        <f aca="false">VLOOKUP(J255,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J255,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13574,8 +13574,8 @@
         <v>3</v>
       </c>
       <c r="K256" s="10" t="n">
-        <f aca="false">VLOOKUP(J256,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J256,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13614,8 +13614,8 @@
         <v>2</v>
       </c>
       <c r="K257" s="10" t="n">
-        <f aca="false">VLOOKUP(J257,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J257,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13654,8 +13654,8 @@
         <v>2</v>
       </c>
       <c r="K258" s="10" t="n">
-        <f aca="false">VLOOKUP(J258,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J258,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13694,8 +13694,8 @@
         <v>2</v>
       </c>
       <c r="K259" s="10" t="n">
-        <f aca="false">VLOOKUP(J259,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J259,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13734,8 +13734,8 @@
         <v>3</v>
       </c>
       <c r="K260" s="10" t="n">
-        <f aca="false">VLOOKUP(J260,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J260,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13774,8 +13774,8 @@
         <v>2</v>
       </c>
       <c r="K261" s="10" t="n">
-        <f aca="false">VLOOKUP(J261,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J261,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13814,8 +13814,8 @@
         <v>2</v>
       </c>
       <c r="K262" s="10" t="n">
-        <f aca="false">VLOOKUP(J262,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J262,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13854,8 +13854,8 @@
         <v>2</v>
       </c>
       <c r="K263" s="10" t="n">
-        <f aca="false">VLOOKUP(J263,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J263,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13894,8 +13894,8 @@
         <v>3</v>
       </c>
       <c r="K264" s="10" t="n">
-        <f aca="false">VLOOKUP(J264,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J264,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13934,8 +13934,8 @@
         <v>3</v>
       </c>
       <c r="K265" s="10" t="n">
-        <f aca="false">VLOOKUP(J265,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J265,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13974,8 +13974,8 @@
         <v>2</v>
       </c>
       <c r="K266" s="10" t="n">
-        <f aca="false">VLOOKUP(J266,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J266,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14014,8 +14014,8 @@
         <v>2</v>
       </c>
       <c r="K267" s="10" t="n">
-        <f aca="false">VLOOKUP(J267,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J267,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14054,8 +14054,8 @@
         <v>2</v>
       </c>
       <c r="K268" s="10" t="n">
-        <f aca="false">VLOOKUP(J268,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J268,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14094,8 +14094,8 @@
         <v>2</v>
       </c>
       <c r="K269" s="10" t="n">
-        <f aca="false">VLOOKUP(J269,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J269,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14134,8 +14134,8 @@
         <v>2</v>
       </c>
       <c r="K270" s="10" t="n">
-        <f aca="false">VLOOKUP(J270,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J270,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14174,8 +14174,8 @@
         <v>3</v>
       </c>
       <c r="K271" s="10" t="n">
-        <f aca="false">VLOOKUP(J271,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J271,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14214,8 +14214,8 @@
         <v>2</v>
       </c>
       <c r="K272" s="10" t="n">
-        <f aca="false">VLOOKUP(J272,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J272,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14254,8 +14254,8 @@
         <v>2</v>
       </c>
       <c r="K273" s="10" t="n">
-        <f aca="false">VLOOKUP(J273,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J273,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14294,8 +14294,8 @@
         <v>3</v>
       </c>
       <c r="K274" s="10" t="n">
-        <f aca="false">VLOOKUP(J274,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J274,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14334,8 +14334,8 @@
         <v>2</v>
       </c>
       <c r="K275" s="10" t="n">
-        <f aca="false">VLOOKUP(J275,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J275,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14374,8 +14374,8 @@
         <v>3</v>
       </c>
       <c r="K276" s="10" t="n">
-        <f aca="false">VLOOKUP(J276,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J276,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14414,8 +14414,8 @@
         <v>2</v>
       </c>
       <c r="K277" s="10" t="n">
-        <f aca="false">VLOOKUP(J277,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J277,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14454,8 +14454,8 @@
         <v>3</v>
       </c>
       <c r="K278" s="10" t="n">
-        <f aca="false">VLOOKUP(J278,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J278,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14494,8 +14494,8 @@
         <v>2</v>
       </c>
       <c r="K279" s="10" t="n">
-        <f aca="false">VLOOKUP(J279,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J279,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14534,8 +14534,8 @@
         <v>3</v>
       </c>
       <c r="K280" s="10" t="n">
-        <f aca="false">VLOOKUP(J280,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J280,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14574,8 +14574,8 @@
         <v>2</v>
       </c>
       <c r="K281" s="10" t="n">
-        <f aca="false">VLOOKUP(J281,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J281,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14614,8 +14614,8 @@
         <v>3</v>
       </c>
       <c r="K282" s="10" t="n">
-        <f aca="false">VLOOKUP(J282,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J282,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14654,8 +14654,8 @@
         <v>3</v>
       </c>
       <c r="K283" s="10" t="n">
-        <f aca="false">VLOOKUP(J283,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J283,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14694,8 +14694,8 @@
         <v>2</v>
       </c>
       <c r="K284" s="10" t="n">
-        <f aca="false">VLOOKUP(J284,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J284,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14734,8 +14734,8 @@
         <v>2</v>
       </c>
       <c r="K285" s="10" t="n">
-        <f aca="false">VLOOKUP(J285,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J285,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14774,8 +14774,8 @@
         <v>2</v>
       </c>
       <c r="K286" s="10" t="n">
-        <f aca="false">VLOOKUP(J286,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J286,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14814,8 +14814,8 @@
         <v>2</v>
       </c>
       <c r="K287" s="10" t="n">
-        <f aca="false">VLOOKUP(J287,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J287,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14854,8 +14854,8 @@
         <v>2</v>
       </c>
       <c r="K288" s="10" t="n">
-        <f aca="false">VLOOKUP(J288,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J288,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14894,8 +14894,8 @@
         <v>2</v>
       </c>
       <c r="K289" s="10" t="n">
-        <f aca="false">VLOOKUP(J289,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J289,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14934,8 +14934,8 @@
         <v>2</v>
       </c>
       <c r="K290" s="10" t="n">
-        <f aca="false">VLOOKUP(J290,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J290,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14974,8 +14974,8 @@
         <v>2</v>
       </c>
       <c r="K291" s="10" t="n">
-        <f aca="false">VLOOKUP(J291,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J291,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15014,8 +15014,8 @@
         <v>2</v>
       </c>
       <c r="K292" s="10" t="n">
-        <f aca="false">VLOOKUP(J292,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J292,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15054,8 +15054,8 @@
         <v>2</v>
       </c>
       <c r="K293" s="10" t="n">
-        <f aca="false">VLOOKUP(J293,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J293,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15094,8 +15094,8 @@
         <v>3</v>
       </c>
       <c r="K294" s="10" t="n">
-        <f aca="false">VLOOKUP(J294,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J294,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15134,8 +15134,8 @@
         <v>1</v>
       </c>
       <c r="K295" s="10" t="n">
-        <f aca="false">VLOOKUP(J295,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.6412093836472</v>
+        <f aca="false">VLOOKUP(J295,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.62684078252735</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15174,8 +15174,8 @@
         <v>3</v>
       </c>
       <c r="K296" s="10" t="n">
-        <f aca="false">VLOOKUP(J296,Summary!$B$3:$G$5,5,0)</f>
-        <v>2.14088958307309</v>
+        <f aca="false">VLOOKUP(J296,Summary!$B$3:$G$5,6,0)</f>
+        <v>2.14085605376106</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15214,8 +15214,8 @@
         <v>2</v>
       </c>
       <c r="K297" s="10" t="n">
-        <f aca="false">VLOOKUP(J297,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J297,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15254,8 +15254,8 @@
         <v>2</v>
       </c>
       <c r="K298" s="10" t="n">
-        <f aca="false">VLOOKUP(J298,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J298,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15294,8 +15294,8 @@
         <v>2</v>
       </c>
       <c r="K299" s="10" t="n">
-        <f aca="false">VLOOKUP(J299,Summary!$B$3:$G$5,5,0)</f>
-        <v>1.92648243951842</v>
+        <f aca="false">VLOOKUP(J299,Summary!$B$3:$G$5,6,0)</f>
+        <v>1.95627068183846</v>
       </c>
     </row>
   </sheetData>

</xml_diff>